<commit_message>
more commits to html tabs
</commit_message>
<xml_diff>
--- a/modules/tabs/docs/templates/Crosstab_Config_Template.xlsx
+++ b/modules/tabs/docs/templates/Crosstab_Config_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/duncan/Documents/Turas/modules/tabs/docs/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32227E33-0EC5-2D46-AE35-BB7C4BCD7942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E583691-4E5E-F141-83D4-A356D93C8CD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="24880" windowHeight="26120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8860" yWindow="500" windowWidth="24880" windowHeight="26120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="263">
   <si>
     <t>Crosstab Configuration Template - Instructions</t>
   </si>
@@ -1037,12 +1037,27 @@
   <si>
     <t>NPS or NPS score</t>
   </si>
+  <si>
+    <t>index_descriptor</t>
+  </si>
+  <si>
+    <t>Strongly disagree(1) = 1 to Strongly agree(5) = 5</t>
+  </si>
+  <si>
+    <t>add the text decriptor of your likert index</t>
+  </si>
+  <si>
+    <t>show_charts</t>
+  </si>
+  <si>
+    <t>TRUE</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1119,12 +1134,6 @@
       <sz val="14"/>
       <color rgb="FF3D3D3A"/>
       <name val="Helvetica"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <color rgb="FF8A2424"/>
-      <name val="Menlo"/>
       <family val="2"/>
     </font>
     <font>
@@ -1255,17 +1264,17 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1581,24 +1590,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="26" t="s">
         <v>190</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
@@ -1606,14 +1615,14 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
@@ -1662,10 +1671,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G153"/>
+  <dimension ref="A1:G101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F99" sqref="F99"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66:B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2463,240 +2472,221 @@
       </c>
     </row>
     <row r="62" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A62" s="24" t="s">
+      <c r="A62" s="20" t="s">
         <v>192</v>
       </c>
-      <c r="B62" s="25" t="b">
+      <c r="B62" s="21" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A63" s="24" t="s">
+      <c r="A63" s="20" t="s">
         <v>193</v>
       </c>
-      <c r="B63" s="25" t="s">
+      <c r="B63" s="21" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A64" s="24" t="s">
+      <c r="A64" s="20" t="s">
         <v>194</v>
       </c>
-      <c r="B64" s="25" t="s">
+      <c r="B64" s="21" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A65" s="24" t="s">
+      <c r="A65" s="20" t="s">
         <v>196</v>
       </c>
-      <c r="B65" s="25" t="b">
+      <c r="B65" s="21" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A66" s="24" t="s">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>261</v>
+      </c>
+      <c r="B66" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A67" s="20" t="s">
         <v>197</v>
       </c>
-      <c r="B66" s="25" t="s">
+      <c r="B67" s="21" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A67" s="24" t="s">
+    <row r="68" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A68" s="20" t="s">
         <v>199</v>
       </c>
-      <c r="B67" s="25" t="s">
+      <c r="B68" s="21" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A68" s="24" t="s">
+    <row r="69" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A69" s="20" t="s">
         <v>201</v>
       </c>
-      <c r="B68" s="25">
+      <c r="B69" s="21">
         <v>100</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A69" s="24" t="s">
+    <row r="70" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A70" s="20" t="s">
         <v>202</v>
       </c>
-      <c r="B69" s="25">
+      <c r="B70" s="21">
         <v>80</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A70" s="24" t="s">
+    <row r="71" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A71" s="20" t="s">
         <v>203</v>
       </c>
-      <c r="B70" s="25">
+      <c r="B71" s="21">
         <v>60</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A71" s="24" t="s">
+    <row r="72" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A72" s="20" t="s">
         <v>204</v>
       </c>
-      <c r="B71" s="25">
+      <c r="B72" s="21">
         <v>80</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A72" s="24" t="s">
+    <row r="73" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A73" s="20" t="s">
         <v>205</v>
       </c>
-      <c r="B72" s="25">
+      <c r="B73" s="21">
         <v>60</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A74" s="4" t="s">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>258</v>
+      </c>
+      <c r="B74" t="s">
+        <v>259</v>
+      </c>
+      <c r="D74" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A76" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B74" s="4" t="s">
+      <c r="B76" s="4" t="s">
         <v>206</v>
-      </c>
-      <c r="C74" s="4"/>
-      <c r="D74" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="E74" s="9"/>
-      <c r="F74" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="G74" s="9" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" ht="64" x14ac:dyDescent="0.2">
-      <c r="A75" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="B75" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="C75" s="4"/>
-      <c r="D75" s="9" t="s">
-        <v>209</v>
-      </c>
-      <c r="E75" s="9"/>
-      <c r="F75" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="G75" s="9" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" ht="70" x14ac:dyDescent="0.2">
-      <c r="A76" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="B76" s="4">
-        <v>10</v>
       </c>
       <c r="C76" s="4"/>
       <c r="D76" s="9" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="E76" s="9"/>
       <c r="F76" s="9" t="s">
-        <v>214</v>
+        <v>143</v>
       </c>
       <c r="G76" s="9" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" ht="70" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="B77" s="4">
-        <v>10</v>
+        <v>199</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>208</v>
       </c>
       <c r="C77" s="4"/>
       <c r="D77" s="9" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="E77" s="9"/>
       <c r="F77" s="9" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="G77" s="9" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="70" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
-        <v>202</v>
+        <v>212</v>
       </c>
       <c r="B78" s="4">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="C78" s="4"/>
       <c r="D78" s="9" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="E78" s="9"/>
       <c r="F78" s="9" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="G78" s="9" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="70" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B79" s="4">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C79" s="4"/>
       <c r="D79" s="9" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E79" s="9"/>
       <c r="F79" s="9" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="G79" s="9" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="70" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
-        <v>223</v>
+        <v>202</v>
       </c>
       <c r="B80" s="4">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="C80" s="4"/>
       <c r="D80" s="9" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="E80" s="9"/>
       <c r="F80" s="9" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="G80" s="9" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7" ht="70" x14ac:dyDescent="0.2">
       <c r="A81" s="4" t="s">
-        <v>226</v>
+        <v>203</v>
       </c>
       <c r="B81" s="4">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C81" s="4"/>
       <c r="D81" s="9" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="E81" s="9"/>
       <c r="F81" s="9" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="G81" s="9" t="s">
         <v>222</v>
@@ -2704,14 +2694,14 @@
     </row>
     <row r="82" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A82" s="4" t="s">
-        <v>204</v>
+        <v>223</v>
       </c>
       <c r="B82" s="4">
         <v>7</v>
       </c>
       <c r="C82" s="4"/>
       <c r="D82" s="9" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="E82" s="9"/>
       <c r="F82" s="9" t="s">
@@ -2723,14 +2713,14 @@
     </row>
     <row r="83" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A83" s="4" t="s">
-        <v>205</v>
+        <v>226</v>
       </c>
       <c r="B83" s="4">
         <v>5</v>
       </c>
       <c r="C83" s="4"/>
       <c r="D83" s="9" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E83" s="9"/>
       <c r="F83" s="9" t="s">
@@ -2740,55 +2730,81 @@
         <v>222</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="70" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A84" s="4" t="s">
-        <v>230</v>
+        <v>204</v>
       </c>
       <c r="B84" s="4">
-        <v>60</v>
+        <v>7</v>
       </c>
       <c r="C84" s="4"/>
       <c r="D84" s="9" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="E84" s="9"/>
       <c r="F84" s="9" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="G84" s="9" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="70" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="s">
-        <v>233</v>
+        <v>205</v>
       </c>
       <c r="B85" s="4">
-        <v>60</v>
+        <v>5</v>
       </c>
       <c r="C85" s="4"/>
       <c r="D85" s="9" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E85" s="9"/>
       <c r="F85" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="G85" s="9" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" ht="70" x14ac:dyDescent="0.2">
+      <c r="A86" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="B86" s="4">
+        <v>60</v>
+      </c>
+      <c r="C86" s="4"/>
+      <c r="D86" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="E86" s="9"/>
+      <c r="F86" s="9" t="s">
         <v>232</v>
       </c>
-      <c r="G85" s="9" t="s">
+      <c r="G86" s="9" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D86" s="9"/>
-      <c r="E86" s="9"/>
-      <c r="F86" s="9"/>
-      <c r="G86" s="9"/>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D87" s="9"/>
+    <row r="87" spans="1:7" ht="70" x14ac:dyDescent="0.2">
+      <c r="A87" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="B87" s="4">
+        <v>60</v>
+      </c>
+      <c r="C87" s="4"/>
+      <c r="D87" s="9" t="s">
+        <v>231</v>
+      </c>
       <c r="E87" s="9"/>
-      <c r="F87" s="9"/>
-      <c r="G87" s="9"/>
+      <c r="F87" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="G87" s="9" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D88" s="9"/>
@@ -2808,159 +2824,130 @@
       <c r="F90" s="9"/>
       <c r="G90" s="9"/>
     </row>
-    <row r="91" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="D91" s="9" t="s">
-        <v>234</v>
-      </c>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D91" s="9"/>
       <c r="E91" s="9"/>
       <c r="F91" s="9"/>
       <c r="G91" s="9"/>
     </row>
-    <row r="92" spans="1:7" ht="38" x14ac:dyDescent="0.2">
-      <c r="D92" s="9" t="s">
-        <v>235</v>
-      </c>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D92" s="9"/>
       <c r="E92" s="9"/>
       <c r="F92" s="9"/>
       <c r="G92" s="9"/>
     </row>
-    <row r="93" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="D93" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="E93" s="9"/>
+      <c r="F93" s="9"/>
+      <c r="G93" s="9"/>
+    </row>
+    <row r="94" spans="1:7" ht="38" x14ac:dyDescent="0.2">
+      <c r="D94" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="E94" s="9"/>
+      <c r="F94" s="9"/>
+      <c r="G94" s="9"/>
+    </row>
+    <row r="95" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="D95" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E93" s="9" t="s">
+      <c r="E95" s="9" t="s">
         <v>236</v>
       </c>
-      <c r="F93" s="9" t="s">
+      <c r="F95" s="9" t="s">
         <v>237</v>
       </c>
-      <c r="G93" s="9" t="s">
+      <c r="G95" s="9" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="94" spans="1:7" ht="144" x14ac:dyDescent="0.2">
-      <c r="D94" s="9" t="s">
+    <row r="96" spans="1:7" ht="144" x14ac:dyDescent="0.2">
+      <c r="D96" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="E94" s="9" t="s">
+      <c r="E96" s="9" t="s">
         <v>239</v>
       </c>
-      <c r="F94" s="9" t="s">
+      <c r="F96" s="9" t="s">
         <v>240</v>
       </c>
-      <c r="G94" s="9" t="s">
+      <c r="G96" s="9" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="95" spans="1:7" ht="128" x14ac:dyDescent="0.2">
-      <c r="D95" s="9" t="s">
+    <row r="97" spans="4:7" ht="128" x14ac:dyDescent="0.2">
+      <c r="D97" s="9" t="s">
         <v>242</v>
       </c>
-      <c r="E95" s="9" t="s">
+      <c r="E97" s="9" t="s">
         <v>243</v>
       </c>
-      <c r="F95" s="9" t="s">
+      <c r="F97" s="9" t="s">
         <v>244</v>
       </c>
-      <c r="G95" s="9" t="s">
+      <c r="G97" s="9" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="106" x14ac:dyDescent="0.2">
-      <c r="D96" s="9" t="s">
+    <row r="98" spans="4:7" ht="106" x14ac:dyDescent="0.2">
+      <c r="D98" s="9" t="s">
         <v>245</v>
       </c>
-      <c r="E96" s="9" t="s">
+      <c r="E98" s="9" t="s">
         <v>246</v>
       </c>
-      <c r="F96" s="9" t="s">
+      <c r="F98" s="9" t="s">
         <v>247</v>
       </c>
-      <c r="G96" s="9" t="s">
+      <c r="G98" s="9" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="97" spans="4:7" ht="106" x14ac:dyDescent="0.2">
-      <c r="D97" s="9" t="s">
+    <row r="99" spans="4:7" ht="106" x14ac:dyDescent="0.2">
+      <c r="D99" s="9" t="s">
         <v>249</v>
       </c>
-      <c r="E97" s="9" t="s">
+      <c r="E99" s="9" t="s">
         <v>250</v>
       </c>
-      <c r="F97" s="9" t="s">
+      <c r="F99" s="9" t="s">
         <v>247</v>
       </c>
-      <c r="G97" s="9" t="s">
+      <c r="G99" s="9" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="98" spans="4:7" ht="120" x14ac:dyDescent="0.2">
-      <c r="D98" s="9" t="s">
+    <row r="100" spans="4:7" ht="120" x14ac:dyDescent="0.2">
+      <c r="D100" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="E98" s="9" t="s">
+      <c r="E100" s="9" t="s">
         <v>253</v>
       </c>
-      <c r="F98" s="9" t="s">
+      <c r="F100" s="9" t="s">
         <v>254</v>
       </c>
-      <c r="G98" s="9" t="s">
+      <c r="G100" s="9" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="99" spans="4:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="D99" s="26" t="s">
+    <row r="101" spans="4:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="D101" s="22" t="s">
         <v>257</v>
       </c>
-      <c r="E99" s="9"/>
-      <c r="F99" s="9" t="s">
+      <c r="E101" s="9"/>
+      <c r="F101" s="9" t="s">
         <v>254</v>
       </c>
-      <c r="G99" s="9" t="s">
+      <c r="G101" s="9" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="113" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="114" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="115" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="116" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="117" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="118" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="119" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="120" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="121" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="122" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="123" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="124" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="125" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="126" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="127" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="128" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="129" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="130" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="131" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="132" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="133" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="134" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="135" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="136" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="137" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="138" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="139" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="140" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="141" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="142" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="143" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="144" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="145" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="146" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="147" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="148" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="149" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="150" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="151" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="152" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="153" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <autoFilter ref="A2:D60" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>